<commit_message>
Changes made to display foundation gridview
</commit_message>
<xml_diff>
--- a/CPSFinal/CPSFinal/DefaultPDF's/UHCL_EM_ACTIVE_COURSE_CATALOG_7133.xlsx
+++ b/CPSFinal/CPSFinal/DefaultPDF's/UHCL_EM_ACTIVE_COURSE_CATALOG_7133.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alira\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alira\Source\Repos\Candidate_Plan_of_Study_Web_Application3\CPSFinal\CPSFinal\DefaultPDF's\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8124" uniqueCount="2946">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8124" uniqueCount="2947">
   <si>
     <t>Subject</t>
   </si>
@@ -8860,6 +8860,9 @@
   </si>
   <si>
     <t>F</t>
+  </si>
+  <si>
+    <t>FOUN</t>
   </si>
 </sst>
 </file>
@@ -9246,8 +9249,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:BJ2683"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A737" sqref="A737"/>
+    <sheetView tabSelected="1" topLeftCell="G790" workbookViewId="0">
+      <selection activeCell="U809" sqref="U809"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -20472,7 +20475,7 @@
         <v>3</v>
       </c>
       <c r="U736" s="5" t="s">
-        <v>2945</v>
+        <v>2946</v>
       </c>
     </row>
     <row r="737" spans="1:21" x14ac:dyDescent="0.35">
@@ -20531,7 +20534,7 @@
         <v>3</v>
       </c>
       <c r="U740" s="5" t="s">
-        <v>2945</v>
+        <v>2946</v>
       </c>
     </row>
     <row r="741" spans="1:21" x14ac:dyDescent="0.35">
@@ -20660,7 +20663,7 @@
         <v>3</v>
       </c>
       <c r="U749" s="5" t="s">
-        <v>2945</v>
+        <v>2946</v>
       </c>
     </row>
     <row r="750" spans="1:21" x14ac:dyDescent="0.35">
@@ -20705,7 +20708,7 @@
         <v>3</v>
       </c>
       <c r="U752" s="5" t="s">
-        <v>2945</v>
+        <v>2946</v>
       </c>
     </row>
     <row r="753" spans="1:21" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Added new code for newstudent page
</commit_message>
<xml_diff>
--- a/CPSFinal/CPSFinal/DefaultPDF's/UHCL_EM_ACTIVE_COURSE_CATALOG_7133.xlsx
+++ b/CPSFinal/CPSFinal/DefaultPDF's/UHCL_EM_ACTIVE_COURSE_CATALOG_7133.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8124" uniqueCount="2947">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8124" uniqueCount="2948">
   <si>
     <t>Subject</t>
   </si>
@@ -8863,6 +8863,9 @@
   </si>
   <si>
     <t>FOUN</t>
+  </si>
+  <si>
+    <t>CORE</t>
   </si>
 </sst>
 </file>
@@ -9249,8 +9252,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:BJ2683"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G790" workbookViewId="0">
-      <selection activeCell="U809" sqref="U809"/>
+    <sheetView tabSelected="1" topLeftCell="A2749" workbookViewId="0">
+      <selection activeCell="A2768" sqref="A2768"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -20935,7 +20938,7 @@
         <v>3</v>
       </c>
       <c r="U768" s="5" t="s">
-        <v>2943</v>
+        <v>2947</v>
       </c>
     </row>
     <row r="769" spans="1:21" x14ac:dyDescent="0.35">
@@ -20980,7 +20983,7 @@
         <v>3</v>
       </c>
       <c r="U771" s="5" t="s">
-        <v>2943</v>
+        <v>2947</v>
       </c>
     </row>
     <row r="772" spans="1:21" x14ac:dyDescent="0.35">
@@ -21011,7 +21014,7 @@
         <v>3</v>
       </c>
       <c r="U773" s="5" t="s">
-        <v>2943</v>
+        <v>2947</v>
       </c>
     </row>
     <row r="774" spans="1:21" x14ac:dyDescent="0.35">
@@ -21126,7 +21129,7 @@
         <v>3</v>
       </c>
       <c r="U781" s="5" t="s">
-        <v>2943</v>
+        <v>2947</v>
       </c>
     </row>
     <row r="782" spans="1:21" x14ac:dyDescent="0.35">

</xml_diff>